<commit_message>
Allow a cell url string to be overwritten.
Separated write_url() hyperlink from the cell data so the cell url
string to be overwritten with a number or formula using a second
write() call to the same cell. The url remains intact. Issue #48.
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/optimize03.xlsx
+++ b/t/regression/xlsx_files/optimize03.xlsx
@@ -11,14 +11,6 @@
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>http://www.perl.com/</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,8 +487,10 @@
           <t>Hyperlinks</t>
         </is>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>0</v>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>http://www.perl.com/</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>